<commit_message>
Updated the PCB - tidied up the libraries
</commit_message>
<xml_diff>
--- a/Hardware/Artemis_Iridium_Tracker_BOM.xlsx
+++ b/Hardware/Artemis_Iridium_Tracker_BOM.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Artemis_Iridium_Tracker" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Artemis_Iridium_Tracker!$A$1:$L$137</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Artemis_Iridium_Tracker!$A$1:$L$134</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="378">
   <si>
     <t>X</t>
   </si>
@@ -945,18 +945,6 @@
     <t>Artemis Module</t>
   </si>
   <si>
-    <t>SOT23-3</t>
-  </si>
-  <si>
-    <t>MCP111T-240E/TT</t>
-  </si>
-  <si>
-    <t>1627192</t>
-  </si>
-  <si>
-    <t>Reset Supervisor; SOT23-3; 2.40V; Open Drain; Active Low</t>
-  </si>
-  <si>
     <t>3.2x1.5</t>
   </si>
   <si>
@@ -1098,12 +1086,6 @@
     <t>M1600HCT-P-SMA</t>
   </si>
   <si>
-    <t>Select on test (may be required for solar power):</t>
-  </si>
-  <si>
-    <t>U11</t>
-  </si>
-  <si>
     <t>AP2112K-3.3TRG1</t>
   </si>
   <si>
@@ -1138,6 +1120,42 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>SSOP3</t>
+  </si>
+  <si>
+    <t>Reset Supervisor; SSOP3; 2.40V; Open Drain; Active Low</t>
+  </si>
+  <si>
+    <t>BD48K24G-TL</t>
+  </si>
+  <si>
+    <t>755-BD48K24G-TL</t>
+  </si>
+  <si>
+    <t>3011055</t>
+  </si>
+  <si>
+    <t>2497607</t>
+  </si>
+  <si>
+    <t>1332158</t>
+  </si>
+  <si>
+    <t>2748850</t>
+  </si>
+  <si>
+    <t>1753762</t>
+  </si>
+  <si>
+    <t>2776798</t>
+  </si>
+  <si>
+    <t>9492615</t>
   </si>
 </sst>
 </file>
@@ -2004,9 +2022,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L138"/>
+  <dimension ref="A1:L135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2145,10 +2165,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="7">
-        <v>50.16</v>
+        <v>50.04</v>
       </c>
       <c r="C7" s="7">
-        <v>0.64</v>
+        <v>0.76</v>
       </c>
       <c r="D7" s="8">
         <v>0</v>
@@ -2169,10 +2189,10 @@
         <v>14</v>
       </c>
       <c r="B8" s="7">
-        <v>0.64</v>
+        <v>0.76</v>
       </c>
       <c r="C8" s="7">
-        <v>62.87</v>
+        <v>62.74</v>
       </c>
       <c r="D8" s="8">
         <v>0</v>
@@ -2777,10 +2797,10 @@
         <v>188</v>
       </c>
       <c r="B28" s="7">
-        <v>24.51</v>
+        <v>24</v>
       </c>
       <c r="C28" s="7">
-        <v>34.04</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="D28" s="8">
         <v>270</v>
@@ -2811,13 +2831,13 @@
         <v>189</v>
       </c>
       <c r="B29" s="7">
-        <v>23.24</v>
+        <v>21.46</v>
       </c>
       <c r="C29" s="7">
-        <v>37.590000000000003</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="D29" s="8">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>56</v>
@@ -2845,10 +2865,10 @@
         <v>190</v>
       </c>
       <c r="B30" s="7">
-        <v>19.100000000000001</v>
+        <v>18.47</v>
       </c>
       <c r="C30" s="7">
-        <v>32.590000000000003</v>
+        <v>32.72</v>
       </c>
       <c r="D30" s="8">
         <v>0</v>
@@ -2913,7 +2933,7 @@
         <v>193</v>
       </c>
       <c r="B32" s="7">
-        <v>19.100000000000001</v>
+        <v>18.47</v>
       </c>
       <c r="C32" s="7">
         <v>35.76</v>
@@ -2947,10 +2967,10 @@
         <v>194</v>
       </c>
       <c r="B33" s="7">
-        <v>19.05</v>
+        <v>18.41</v>
       </c>
       <c r="C33" s="7">
-        <v>34.159999999999997</v>
+        <v>34.29</v>
       </c>
       <c r="D33" s="8">
         <v>180</v>
@@ -3347,10 +3367,10 @@
         <v>228</v>
       </c>
       <c r="B45" s="7">
-        <v>32.64</v>
+        <v>32</v>
       </c>
       <c r="C45" s="7">
-        <v>11.56</v>
+        <v>12.19</v>
       </c>
       <c r="D45" s="8">
         <v>180</v>
@@ -3702,7 +3722,7 @@
         <v>10.79</v>
       </c>
       <c r="C56" s="7">
-        <v>4.01</v>
+        <v>3.76</v>
       </c>
       <c r="D56" s="8">
         <v>0</v>
@@ -3710,16 +3730,16 @@
       <c r="E56" s="8"/>
       <c r="F56" s="9"/>
       <c r="G56" s="6" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="I56" s="9"/>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
       <c r="L56" s="6" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -3745,7 +3765,9 @@
       <c r="H57" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="I57" s="9"/>
+      <c r="I57" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="J57" s="6"/>
       <c r="K57" s="6" t="s">
         <v>256</v>
@@ -3777,7 +3799,9 @@
       <c r="H58" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="I58" s="9"/>
+      <c r="I58" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="J58" s="6"/>
       <c r="K58" s="6" t="s">
         <v>256</v>
@@ -3794,7 +3818,7 @@
         <v>37.590000000000003</v>
       </c>
       <c r="C59" s="7">
-        <v>50.8</v>
+        <v>50.16</v>
       </c>
       <c r="D59" s="8">
         <v>90</v>
@@ -3828,7 +3852,7 @@
         <v>41.4</v>
       </c>
       <c r="C60" s="7">
-        <v>48.03</v>
+        <v>48.01</v>
       </c>
       <c r="D60" s="8">
         <v>270</v>
@@ -3843,7 +3867,9 @@
       <c r="H60" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="I60" s="9"/>
+      <c r="I60" s="9" t="s">
+        <v>376</v>
+      </c>
       <c r="J60" s="6"/>
       <c r="K60" s="6" t="s">
         <v>272</v>
@@ -3863,7 +3889,7 @@
         <v>49.28</v>
       </c>
       <c r="D61" s="8">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>69</v>
@@ -3962,7 +3988,7 @@
         <v>37.340000000000003</v>
       </c>
       <c r="C64" s="7">
-        <v>33.020000000000003</v>
+        <v>33.07</v>
       </c>
       <c r="D64" s="8">
         <v>0</v>
@@ -4139,21 +4165,21 @@
         <v>56</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="G69" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="I69" s="9" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
       <c r="L69" s="6" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -4513,21 +4539,21 @@
         <v>56</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="G80" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H80" s="9" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="I80" s="9" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="J80" s="6"/>
       <c r="K80" s="6"/>
       <c r="L80" s="6" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -4615,21 +4641,21 @@
         <v>56</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="G83" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H83" s="9" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="I83" s="9" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="J83" s="6"/>
       <c r="K83" s="6"/>
       <c r="L83" s="6" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -4751,21 +4777,21 @@
         <v>56</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="G87" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H87" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="I87" s="9" t="s">
         <v>340</v>
-      </c>
-      <c r="I87" s="9" t="s">
-        <v>344</v>
       </c>
       <c r="J87" s="6"/>
       <c r="K87" s="6"/>
       <c r="L87" s="6" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
@@ -4853,21 +4879,21 @@
         <v>56</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="G90" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H90" s="9" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="I90" s="9" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="J90" s="6"/>
       <c r="K90" s="6"/>
       <c r="L90" s="6" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
@@ -4887,21 +4913,21 @@
         <v>56</v>
       </c>
       <c r="F91" s="9" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G91" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H91" s="9" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="I91" s="9" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="J91" s="6"/>
       <c r="K91" s="6"/>
       <c r="L91" s="6" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
@@ -4988,18 +5014,18 @@
       <c r="E94" s="8"/>
       <c r="F94" s="9"/>
       <c r="G94" s="6" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="H94" s="9" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="I94" s="9"/>
       <c r="J94" s="6"/>
       <c r="K94" s="6" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="L94" s="6" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
@@ -5016,11 +5042,11 @@
         <v>90</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="F95" s="9"/>
       <c r="G95" s="6" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="H95" s="9" t="s">
         <v>297</v>
@@ -5029,7 +5055,7 @@
       <c r="J95" s="6"/>
       <c r="K95" s="6"/>
       <c r="L95" s="6" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
@@ -5120,7 +5146,7 @@
         <v>298</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="H98" s="9" t="s">
         <v>298</v>
@@ -5129,7 +5155,7 @@
       <c r="J98" s="6"/>
       <c r="K98" s="6"/>
       <c r="L98" s="16" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
@@ -5157,7 +5183,9 @@
       <c r="H99" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="I99" s="9"/>
+      <c r="I99" s="9" t="s">
+        <v>375</v>
+      </c>
       <c r="J99" s="6"/>
       <c r="K99" s="6" t="s">
         <v>303</v>
@@ -5185,15 +5213,17 @@
         <v>299</v>
       </c>
       <c r="H100" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="I100" s="9"/>
+        <v>320</v>
+      </c>
+      <c r="I100" s="9" t="s">
+        <v>374</v>
+      </c>
       <c r="J100" s="6"/>
       <c r="K100" s="6" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="L100" s="6" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
@@ -5220,232 +5250,258 @@
       <c r="I101" s="9"/>
       <c r="J101" s="6"/>
       <c r="K101" s="6" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="L101" s="16" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
-        <v>293</v>
+        <v>366</v>
       </c>
       <c r="B102" s="7">
-        <v>22.48</v>
+        <v>13.97</v>
       </c>
       <c r="C102" s="7">
-        <v>11.81</v>
+        <v>31.29</v>
       </c>
       <c r="D102" s="8">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>321</v>
+        <v>367</v>
       </c>
       <c r="F102" s="9" t="s">
-        <v>318</v>
+        <v>369</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>78</v>
+        <v>242</v>
       </c>
       <c r="H102" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="I102" s="9"/>
+        <v>369</v>
+      </c>
+      <c r="I102" s="9" t="s">
+        <v>371</v>
+      </c>
       <c r="J102" s="6"/>
       <c r="K102" s="6" t="s">
-        <v>319</v>
+        <v>370</v>
       </c>
       <c r="L102" s="6" t="s">
-        <v>320</v>
+        <v>368</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
-        <v>359</v>
+        <v>293</v>
       </c>
       <c r="B103" s="7">
-        <v>5.33</v>
+        <v>22.48</v>
       </c>
       <c r="C103" s="7">
-        <v>33.659999999999997</v>
+        <v>12.7</v>
       </c>
       <c r="D103" s="8">
         <v>270</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>360</v>
+        <v>314</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="H103" s="9" t="s">
-        <v>360</v>
+        <v>314</v>
       </c>
       <c r="I103" s="9" t="s">
-        <v>362</v>
+        <v>373</v>
       </c>
       <c r="J103" s="6"/>
       <c r="K103" s="6" t="s">
-        <v>363</v>
+        <v>315</v>
       </c>
       <c r="L103" s="6" t="s">
-        <v>361</v>
+        <v>316</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B104" s="7">
-        <v>22.48</v>
+        <v>5.33</v>
       </c>
       <c r="C104" s="7">
-        <v>34.29</v>
+        <v>33.659999999999997</v>
       </c>
       <c r="D104" s="8">
         <v>270</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="F104" s="9">
-        <v>32.768000000000001</v>
+        <v>317</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>312</v>
+        <v>70</v>
       </c>
       <c r="H104" s="9" t="s">
-        <v>313</v>
+        <v>354</v>
       </c>
       <c r="I104" s="9" t="s">
-        <v>314</v>
+        <v>356</v>
       </c>
       <c r="J104" s="6"/>
-      <c r="K104" s="6"/>
+      <c r="K104" s="6" t="s">
+        <v>357</v>
+      </c>
       <c r="L104" s="6" t="s">
-        <v>315</v>
+        <v>355</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B105" s="7">
-        <v>45.85</v>
+        <v>22.73</v>
       </c>
       <c r="C105" s="7">
-        <v>45.21</v>
+        <v>33.15</v>
       </c>
       <c r="D105" s="8">
         <v>0</v>
       </c>
       <c r="E105" s="8" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F105" s="9">
         <v>32.768000000000001</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="H105" s="9" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="I105" s="9" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="J105" s="6"/>
       <c r="K105" s="6"/>
       <c r="L105" s="6" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="B106" s="12">
-        <v>12.9</v>
-      </c>
-      <c r="C106" s="12">
-        <v>22.86</v>
-      </c>
-      <c r="D106" s="11" t="s">
-        <v>371</v>
-      </c>
-      <c r="E106" s="11"/>
-      <c r="F106" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="G106" s="11" t="s">
-        <v>367</v>
-      </c>
-      <c r="H106" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="I106" s="13"/>
-      <c r="J106" s="11"/>
-      <c r="K106" s="11" t="s">
-        <v>369</v>
-      </c>
-      <c r="L106" s="11" t="s">
-        <v>370</v>
+        <v>296</v>
+      </c>
+      <c r="B106" s="7">
+        <v>45.85</v>
+      </c>
+      <c r="C106" s="7">
+        <v>45.21</v>
+      </c>
+      <c r="D106" s="8">
+        <v>0</v>
+      </c>
+      <c r="E106" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="F106" s="9">
+        <v>32.768000000000001</v>
+      </c>
+      <c r="G106" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="H106" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="I106" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="J106" s="6"/>
+      <c r="K106" s="6"/>
+      <c r="L106" s="6" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="107" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B107" s="12">
-        <v>37.9</v>
+        <v>12.9</v>
       </c>
       <c r="C107" s="12">
         <v>22.86</v>
       </c>
       <c r="D107" s="11" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="E107" s="11"/>
       <c r="F107" s="13" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="G107" s="11" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="H107" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="I107" s="13"/>
+        <v>362</v>
+      </c>
+      <c r="I107" s="13" t="s">
+        <v>372</v>
+      </c>
       <c r="J107" s="11"/>
       <c r="K107" s="11" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L107" s="11" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A108" s="11"/>
-      <c r="B108" s="7"/>
-      <c r="C108" s="7"/>
-      <c r="D108" s="8"/>
-      <c r="E108" s="8"/>
-      <c r="F108" s="9"/>
-      <c r="G108" s="6"/>
-      <c r="H108" s="9"/>
-      <c r="I108" s="9"/>
-      <c r="J108" s="6"/>
-      <c r="K108" s="6"/>
-      <c r="L108" s="6"/>
+        <v>364</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B108" s="12">
+        <v>37.9</v>
+      </c>
+      <c r="C108" s="12">
+        <v>22.86</v>
+      </c>
+      <c r="D108" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="E108" s="11"/>
+      <c r="F108" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="G108" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="H108" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="I108" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="J108" s="11"/>
+      <c r="K108" s="11" t="s">
+        <v>363</v>
+      </c>
+      <c r="L108" s="11" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>358</v>
-      </c>
+      <c r="A109" s="11"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="8"/>
@@ -5459,181 +5515,169 @@
       <c r="L109" s="6"/>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
-      <c r="B110" s="7"/>
-      <c r="C110" s="7"/>
-      <c r="D110" s="8"/>
-      <c r="E110" s="8"/>
-      <c r="F110" s="9"/>
+      <c r="A110" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B110" s="9"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="10"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="6"/>
       <c r="G110" s="6"/>
-      <c r="H110" s="9"/>
-      <c r="I110" s="9"/>
-      <c r="J110" s="6"/>
-      <c r="K110" s="6"/>
-      <c r="L110" s="6"/>
+      <c r="H110" s="6"/>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A111" s="11" t="s">
-        <v>294</v>
-      </c>
-      <c r="B111" s="7">
-        <v>14.61</v>
-      </c>
-      <c r="C111" s="7">
-        <v>29.85</v>
-      </c>
-      <c r="D111" s="8">
-        <v>90</v>
-      </c>
-      <c r="E111" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="F111" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="G111" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H111" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="I111" s="9" t="s">
-        <v>309</v>
-      </c>
-      <c r="J111" s="6"/>
-      <c r="K111" s="6"/>
-      <c r="L111" s="6" t="s">
-        <v>310</v>
-      </c>
+      <c r="A111" s="1"/>
+      <c r="B111" s="9"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="10"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A112" s="11"/>
-      <c r="B112" s="7"/>
-      <c r="C112" s="7"/>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8"/>
-      <c r="F112" s="9"/>
-      <c r="G112" s="6"/>
-      <c r="H112" s="9"/>
-      <c r="I112" s="9"/>
-      <c r="J112" s="6"/>
-      <c r="K112" s="6"/>
-      <c r="L112" s="6"/>
+      <c r="A112" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B112" s="9"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G112" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H112" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="I112" t="s">
+        <v>120</v>
+      </c>
+      <c r="L112" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B113" s="9"/>
-      <c r="C113" s="6"/>
-      <c r="D113" s="10"/>
+      <c r="A113" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B113" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="C113" s="21"/>
+      <c r="D113" s="21"/>
       <c r="E113" s="9"/>
-      <c r="F113" s="6"/>
-      <c r="G113" s="6"/>
-      <c r="H113" s="6"/>
+      <c r="F113" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G113" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H113" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I113" t="s">
+        <v>53</v>
+      </c>
+      <c r="L113" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-      <c r="B114" s="9"/>
+      <c r="A114" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B114" s="6"/>
       <c r="C114" s="6"/>
-      <c r="D114" s="10"/>
+      <c r="D114" s="6"/>
       <c r="E114" s="9"/>
-      <c r="F114" s="6"/>
-      <c r="G114" s="6"/>
-      <c r="H114" s="6"/>
+      <c r="F114" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G114" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H114" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="I114" s="17">
+        <v>2856818</v>
+      </c>
+      <c r="L114" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A115" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B115" s="9"/>
+      <c r="A115" s="6"/>
+      <c r="B115" s="6"/>
       <c r="C115" s="6"/>
-      <c r="D115" s="10"/>
-      <c r="E115" s="9"/>
-      <c r="F115" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="G115" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H115" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="I115" t="s">
-        <v>120</v>
-      </c>
-      <c r="L115" t="s">
-        <v>121</v>
-      </c>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="9"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="9"/>
+      <c r="I115" s="9"/>
+      <c r="J115" s="6"/>
+      <c r="K115" s="6"/>
+      <c r="L115" s="6"/>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A116" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B116" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="C116" s="21"/>
-      <c r="D116" s="21"/>
-      <c r="E116" s="9"/>
-      <c r="F116" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G116" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H116" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="I116" t="s">
-        <v>53</v>
-      </c>
-      <c r="L116" t="s">
-        <v>54</v>
-      </c>
+      <c r="A116" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B116" s="6"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="9"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="9"/>
+      <c r="I116" s="9"/>
+      <c r="J116" s="6"/>
+      <c r="K116" s="6"/>
+      <c r="L116" s="6"/>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A117" s="18" t="s">
-        <v>108</v>
-      </c>
+      <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
       <c r="D117" s="6"/>
-      <c r="E117" s="9"/>
-      <c r="F117" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G117" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H117" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="I117" s="17">
-        <v>2856818</v>
-      </c>
-      <c r="L117" t="s">
-        <v>146</v>
-      </c>
+      <c r="E117" s="6"/>
+      <c r="F117" s="9"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="9"/>
+      <c r="I117" s="9"/>
+      <c r="J117" s="6"/>
+      <c r="K117" s="6"/>
+      <c r="L117" s="6"/>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A118" s="6"/>
+      <c r="A118" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="B118" s="6"/>
       <c r="C118" s="6"/>
       <c r="D118" s="6"/>
       <c r="E118" s="6"/>
       <c r="F118" s="9"/>
-      <c r="G118" s="6"/>
-      <c r="H118" s="9"/>
+      <c r="G118" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H118" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="I118" s="9"/>
       <c r="J118" s="6"/>
       <c r="K118" s="6"/>
-      <c r="L118" s="6"/>
+      <c r="L118" s="16" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="A119" s="6"/>
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
       <c r="D119" s="6"/>
@@ -5647,59 +5691,47 @@
       <c r="L119" s="6"/>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A120" s="6"/>
-      <c r="B120" s="6"/>
+      <c r="A120" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B120" s="9"/>
       <c r="C120" s="6"/>
-      <c r="D120" s="6"/>
-      <c r="E120" s="6"/>
-      <c r="F120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
+      <c r="F120" s="6"/>
       <c r="G120" s="6"/>
-      <c r="H120" s="9"/>
-      <c r="I120" s="9"/>
-      <c r="J120" s="6"/>
-      <c r="K120" s="6"/>
-      <c r="L120" s="6"/>
+      <c r="H120" s="6"/>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A121" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B121" s="6"/>
+      <c r="A121" s="1"/>
+      <c r="B121" s="9"/>
       <c r="C121" s="6"/>
-      <c r="D121" s="6"/>
-      <c r="E121" s="6"/>
-      <c r="F121" s="9"/>
-      <c r="G121" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H121" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I121" s="9"/>
-      <c r="J121" s="6"/>
-      <c r="K121" s="6"/>
-      <c r="L121" s="16" t="s">
-        <v>96</v>
-      </c>
+      <c r="D121" s="9"/>
+      <c r="E121" s="9"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="6"/>
+      <c r="H121" s="6"/>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A122" s="6"/>
-      <c r="B122" s="6"/>
+      <c r="A122" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B122" s="9"/>
       <c r="C122" s="6"/>
-      <c r="D122" s="6"/>
-      <c r="E122" s="6"/>
-      <c r="F122" s="9"/>
+      <c r="D122" s="9"/>
+      <c r="E122" s="9"/>
+      <c r="F122" s="6"/>
       <c r="G122" s="6"/>
-      <c r="H122" s="9"/>
-      <c r="I122" s="9"/>
-      <c r="J122" s="6"/>
-      <c r="K122" s="6"/>
-      <c r="L122" s="6"/>
+      <c r="H122" s="6"/>
+      <c r="J122" t="s">
+        <v>359</v>
+      </c>
+      <c r="L122" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="A123" s="6"/>
       <c r="B123" s="9"/>
       <c r="C123" s="6"/>
       <c r="D123" s="9"/>
@@ -5709,7 +5741,9 @@
       <c r="H123" s="6"/>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
+      <c r="A124" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="B124" s="9"/>
       <c r="C124" s="6"/>
       <c r="D124" s="9"/>
@@ -5719,9 +5753,7 @@
       <c r="H124" s="6"/>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A125" s="6" t="s">
-        <v>47</v>
-      </c>
+      <c r="A125" s="1"/>
       <c r="B125" s="9"/>
       <c r="C125" s="6"/>
       <c r="D125" s="9"/>
@@ -5729,27 +5761,31 @@
       <c r="F125" s="6"/>
       <c r="G125" s="6"/>
       <c r="H125" s="6"/>
-      <c r="J125" t="s">
-        <v>365</v>
-      </c>
-      <c r="L125" t="s">
-        <v>364</v>
-      </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A126" s="6"/>
+      <c r="A126" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="B126" s="9"/>
       <c r="C126" s="6"/>
       <c r="D126" s="9"/>
       <c r="E126" s="9"/>
       <c r="F126" s="6"/>
-      <c r="G126" s="6"/>
-      <c r="H126" s="6"/>
+      <c r="G126" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H126" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I126" s="17">
+        <v>2664624</v>
+      </c>
+      <c r="L126" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="A127" s="6"/>
       <c r="B127" s="9"/>
       <c r="C127" s="6"/>
       <c r="D127" s="9"/>
@@ -5759,7 +5795,9 @@
       <c r="H127" s="6"/>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A128" s="1"/>
+      <c r="A128" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="B128" s="9"/>
       <c r="C128" s="6"/>
       <c r="D128" s="9"/>
@@ -5769,41 +5807,39 @@
       <c r="H128" s="6"/>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A129" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="A129" s="1"/>
       <c r="B129" s="9"/>
       <c r="C129" s="6"/>
       <c r="D129" s="9"/>
       <c r="E129" s="9"/>
       <c r="F129" s="6"/>
-      <c r="G129" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H129" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="I129" s="17">
-        <v>2664624</v>
-      </c>
-      <c r="L129" t="s">
-        <v>95</v>
-      </c>
+      <c r="G129" s="6"/>
+      <c r="H129" s="6"/>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A130" s="6"/>
+      <c r="A130" s="6" t="s">
+        <v>257</v>
+      </c>
       <c r="B130" s="9"/>
       <c r="C130" s="6"/>
       <c r="D130" s="9"/>
       <c r="E130" s="9"/>
       <c r="F130" s="6"/>
-      <c r="G130" s="6"/>
-      <c r="H130" s="6"/>
+      <c r="G130" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H130" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="I130" s="17">
+        <v>2281621</v>
+      </c>
+      <c r="L130" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="A131" s="6"/>
       <c r="B131" s="9"/>
       <c r="C131" s="6"/>
       <c r="D131" s="9"/>
@@ -5813,7 +5849,9 @@
       <c r="H131" s="6"/>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A132" s="1"/>
+      <c r="A132" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="B132" s="9"/>
       <c r="C132" s="6"/>
       <c r="D132" s="9"/>
@@ -5823,29 +5861,19 @@
       <c r="H132" s="6"/>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A133" s="6" t="s">
-        <v>257</v>
-      </c>
+      <c r="A133" s="1"/>
       <c r="B133" s="9"/>
       <c r="C133" s="6"/>
       <c r="D133" s="9"/>
       <c r="E133" s="9"/>
       <c r="F133" s="6"/>
-      <c r="G133" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H133" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="I133" s="17">
-        <v>2281621</v>
-      </c>
-      <c r="L133" t="s">
-        <v>258</v>
-      </c>
+      <c r="G133" s="6"/>
+      <c r="H133" s="6"/>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A134" s="6"/>
+      <c r="A134" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="B134" s="9"/>
       <c r="C134" s="6"/>
       <c r="D134" s="9"/>
@@ -5855,48 +5883,14 @@
       <c r="H134" s="6"/>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B135" s="9"/>
-      <c r="C135" s="6"/>
-      <c r="D135" s="9"/>
-      <c r="E135" s="9"/>
-      <c r="F135" s="6"/>
-      <c r="G135" s="6"/>
-      <c r="H135" s="6"/>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A136" s="1"/>
-      <c r="B136" s="9"/>
-      <c r="C136" s="6"/>
-      <c r="D136" s="9"/>
-      <c r="E136" s="9"/>
-      <c r="F136" s="6"/>
-      <c r="G136" s="6"/>
-      <c r="H136" s="6"/>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A137" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B137" s="9"/>
-      <c r="C137" s="6"/>
-      <c r="D137" s="9"/>
-      <c r="E137" s="9"/>
-      <c r="F137" s="6"/>
-      <c r="G137" s="6"/>
-      <c r="H137" s="6"/>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A138" s="6"/>
+      <c r="A135" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="B113:D113"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="L121" r:id="rId1"/>
+    <hyperlink ref="L118" r:id="rId1"/>
     <hyperlink ref="L98" r:id="rId2"/>
     <hyperlink ref="L101" r:id="rId3"/>
   </hyperlinks>

</xml_diff>